<commit_message>
updated docs - through GFFS
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/EMBARK Lab/Code/bam-bookdown/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Dropbox/Wisconsin/EMBARK Lab/Code/BAM-codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EE896B-ABAC-C147-BC7D-82BE06E74750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D7063B-19A8-2F4A-AC56-9952371836EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1120" windowWidth="27640" windowHeight="16740" xr2:uid="{65510864-A106-F142-86F0-C8E6371AAB60}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>Demographics</t>
   </si>
@@ -94,13 +94,19 @@
     <t>Weight-based Approach Avoidance Task*</t>
   </si>
   <si>
-    <t>Implicit Attitudes Test – Body Size*</t>
-  </si>
-  <si>
     <t>ED History Questionnaire (ED100k after 9/1/2022)</t>
   </si>
   <si>
     <t>ED Fear Questionnaire (after 9/1/2022)</t>
+  </si>
+  <si>
+    <t>Weight Impliciat Association Test (Weight IAT)*</t>
+  </si>
+  <si>
+    <t>ED100k (after 9/1/2022)</t>
+  </si>
+  <si>
+    <t>Eating Disorder Diagnostic Scale (EDDS)</t>
   </si>
 </sst>
 </file>
@@ -533,15 +539,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF68AE7-13CA-AC4E-9604-A56C12406A02}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" style="1" customWidth="1"/>
     <col min="2" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -579,9 +585,9 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -591,85 +597,85 @@
     </row>
     <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3"/>
@@ -677,7 +683,7 @@
     </row>
     <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -685,80 +691,104 @@
       <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
+      <c r="B19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D18">
-    <sortCondition ref="A1:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
+    <sortCondition ref="A1:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>